<commit_message>
add table_chart script with prenorm
</commit_message>
<xml_diff>
--- a/visualization/perplexity_table.xlsx
+++ b/visualization/perplexity_table.xlsx
@@ -463,7 +463,7 @@
         <v>36.7371</v>
       </c>
       <c r="C2" t="n">
-        <v>36.7371</v>
+        <v>33.9126</v>
       </c>
       <c r="D2" t="n">
         <v>36.7371</v>
@@ -477,7 +477,7 @@
         <v>26.8323</v>
       </c>
       <c r="C3" t="n">
-        <v>26.8323</v>
+        <v>26.7691</v>
       </c>
       <c r="D3" t="n">
         <v>26.8323</v>
@@ -491,7 +491,7 @@
         <v>22.725</v>
       </c>
       <c r="C4" t="n">
-        <v>22.725</v>
+        <v>23.2335</v>
       </c>
       <c r="D4" t="n">
         <v>22.725</v>
@@ -505,7 +505,7 @@
         <v>20.6885</v>
       </c>
       <c r="C5" t="n">
-        <v>20.6885</v>
+        <v>20.7174</v>
       </c>
       <c r="D5" t="n">
         <v>20.6885</v>
@@ -519,7 +519,7 @@
         <v>19.0923</v>
       </c>
       <c r="C6" t="n">
-        <v>19.0923</v>
+        <v>18.8327</v>
       </c>
       <c r="D6" t="n">
         <v>19.0923</v>
@@ -533,7 +533,7 @@
         <v>17.8984</v>
       </c>
       <c r="C7" t="n">
-        <v>17.8984</v>
+        <v>17.4664</v>
       </c>
       <c r="D7" t="n">
         <v>17.8984</v>
@@ -547,7 +547,7 @@
         <v>17.2346</v>
       </c>
       <c r="C8" t="n">
-        <v>17.2346</v>
+        <v>16.0299</v>
       </c>
       <c r="D8" t="n">
         <v>17.2346</v>
@@ -561,7 +561,7 @@
         <v>16.2702</v>
       </c>
       <c r="C9" t="n">
-        <v>16.2702</v>
+        <v>14.7069</v>
       </c>
       <c r="D9" t="n">
         <v>16.2702</v>
@@ -575,7 +575,7 @@
         <v>15.4719</v>
       </c>
       <c r="C10" t="n">
-        <v>15.4719</v>
+        <v>13.1254</v>
       </c>
       <c r="D10" t="n">
         <v>15.4719</v>
@@ -589,7 +589,7 @@
         <v>14.5493</v>
       </c>
       <c r="C11" t="n">
-        <v>14.5493</v>
+        <v>12.2506</v>
       </c>
       <c r="D11" t="n">
         <v>14.5493</v>
@@ -603,7 +603,7 @@
         <v>13.5227</v>
       </c>
       <c r="C12" t="n">
-        <v>13.5227</v>
+        <v>11.582</v>
       </c>
       <c r="D12" t="n">
         <v>13.5227</v>
@@ -617,7 +617,7 @@
         <v>12.4982</v>
       </c>
       <c r="C13" t="n">
-        <v>12.4982</v>
+        <v>11.24</v>
       </c>
       <c r="D13" t="n">
         <v>12.4982</v>
@@ -631,7 +631,7 @@
         <v>11.7911</v>
       </c>
       <c r="C14" t="n">
-        <v>11.7911</v>
+        <v>10.8999</v>
       </c>
       <c r="D14" t="n">
         <v>11.7911</v>
@@ -645,7 +645,7 @@
         <v>11.1716</v>
       </c>
       <c r="C15" t="n">
-        <v>11.1716</v>
+        <v>10.4693</v>
       </c>
       <c r="D15" t="n">
         <v>11.1716</v>
@@ -659,7 +659,7 @@
         <v>10.7728</v>
       </c>
       <c r="C16" t="n">
-        <v>10.7728</v>
+        <v>10.2536</v>
       </c>
       <c r="D16" t="n">
         <v>10.7728</v>
@@ -673,7 +673,7 @@
         <v>10.4022</v>
       </c>
       <c r="C17" t="n">
-        <v>10.4022</v>
+        <v>9.966200000000001</v>
       </c>
       <c r="D17" t="n">
         <v>10.4022</v>
@@ -687,7 +687,7 @@
         <v>10.2219</v>
       </c>
       <c r="C18" t="n">
-        <v>10.2219</v>
+        <v>9.8307</v>
       </c>
       <c r="D18" t="n">
         <v>10.2219</v>
@@ -701,7 +701,7 @@
         <v>10.1277</v>
       </c>
       <c r="C19" t="n">
-        <v>10.1277</v>
+        <v>9.6778</v>
       </c>
       <c r="D19" t="n">
         <v>10.1277</v>
@@ -715,7 +715,7 @@
         <v>9.918699999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>9.918699999999999</v>
+        <v>9.592499999999999</v>
       </c>
       <c r="D20" t="n">
         <v>9.918699999999999</v>
@@ -729,7 +729,7 @@
         <v>9.7295</v>
       </c>
       <c r="C21" t="n">
-        <v>9.7295</v>
+        <v>9.424200000000001</v>
       </c>
       <c r="D21" t="n">
         <v>9.7295</v>
@@ -743,7 +743,7 @@
         <v>9.6303</v>
       </c>
       <c r="C22" t="n">
-        <v>9.6303</v>
+        <v>9.3149</v>
       </c>
       <c r="D22" t="n">
         <v>9.6303</v>
@@ -757,7 +757,7 @@
         <v>9.4011</v>
       </c>
       <c r="C23" t="n">
-        <v>9.4011</v>
+        <v>9.076700000000001</v>
       </c>
       <c r="D23" t="n">
         <v>9.4011</v>
@@ -771,7 +771,7 @@
         <v>9.2904</v>
       </c>
       <c r="C24" t="n">
-        <v>9.2904</v>
+        <v>9.058</v>
       </c>
       <c r="D24" t="n">
         <v>9.2904</v>
@@ -785,7 +785,7 @@
         <v>9.214499999999999</v>
       </c>
       <c r="C25" t="n">
-        <v>9.214499999999999</v>
+        <v>8.942299999999999</v>
       </c>
       <c r="D25" t="n">
         <v>9.214499999999999</v>
@@ -799,7 +799,7 @@
         <v>9.0945</v>
       </c>
       <c r="C26" t="n">
-        <v>9.0945</v>
+        <v>8.9269</v>
       </c>
       <c r="D26" t="n">
         <v>9.0945</v>
@@ -813,7 +813,7 @@
         <v>8.9445</v>
       </c>
       <c r="C27" t="n">
-        <v>8.9445</v>
+        <v>8.7235</v>
       </c>
       <c r="D27" t="n">
         <v>8.9445</v>
@@ -827,7 +827,7 @@
         <v>8.965299999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>8.965299999999999</v>
+        <v>8.697900000000001</v>
       </c>
       <c r="D28" t="n">
         <v>8.965299999999999</v>
@@ -841,7 +841,7 @@
         <v>8.859</v>
       </c>
       <c r="C29" t="n">
-        <v>8.859</v>
+        <v>8.5908</v>
       </c>
       <c r="D29" t="n">
         <v>8.859</v>
@@ -855,7 +855,7 @@
         <v>8.7577</v>
       </c>
       <c r="C30" t="n">
-        <v>8.7577</v>
+        <v>8.601100000000001</v>
       </c>
       <c r="D30" t="n">
         <v>8.7577</v>
@@ -869,7 +869,7 @@
         <v>8.667899999999999</v>
       </c>
       <c r="C31" t="n">
-        <v>8.667899999999999</v>
+        <v>8.539</v>
       </c>
       <c r="D31" t="n">
         <v>8.667899999999999</v>
@@ -883,7 +883,7 @@
         <v>8.5959</v>
       </c>
       <c r="C32" t="n">
-        <v>8.5959</v>
+        <v>8.469099999999999</v>
       </c>
       <c r="D32" t="n">
         <v>8.5959</v>
@@ -897,7 +897,7 @@
         <v>8.487500000000001</v>
       </c>
       <c r="C33" t="n">
-        <v>8.487500000000001</v>
+        <v>8.3421</v>
       </c>
       <c r="D33" t="n">
         <v>8.487500000000001</v>
@@ -911,7 +911,7 @@
         <v>8.4442</v>
       </c>
       <c r="C34" t="n">
-        <v>8.4442</v>
+        <v>8.336399999999999</v>
       </c>
       <c r="D34" t="n">
         <v>8.4442</v>
@@ -925,7 +925,7 @@
         <v>8.3749</v>
       </c>
       <c r="C35" t="n">
-        <v>8.3749</v>
+        <v>8.2117</v>
       </c>
       <c r="D35" t="n">
         <v>8.3749</v>
@@ -939,7 +939,7 @@
         <v>8.3592</v>
       </c>
       <c r="C36" t="n">
-        <v>8.3592</v>
+        <v>8.236800000000001</v>
       </c>
       <c r="D36" t="n">
         <v>8.3592</v>
@@ -953,7 +953,7 @@
         <v>8.372</v>
       </c>
       <c r="C37" t="n">
-        <v>8.372</v>
+        <v>8.3376</v>
       </c>
       <c r="D37" t="n">
         <v>8.372</v>
@@ -967,7 +967,7 @@
         <v>8.289899999999999</v>
       </c>
       <c r="C38" t="n">
-        <v>8.289899999999999</v>
+        <v>8.2333</v>
       </c>
       <c r="D38" t="n">
         <v>8.289899999999999</v>
@@ -981,7 +981,7 @@
         <v>8.1881</v>
       </c>
       <c r="C39" t="n">
-        <v>8.1881</v>
+        <v>8.1289</v>
       </c>
       <c r="D39" t="n">
         <v>8.1881</v>
@@ -995,7 +995,7 @@
         <v>8.2098</v>
       </c>
       <c r="C40" t="n">
-        <v>8.2098</v>
+        <v>8.2066</v>
       </c>
       <c r="D40" t="n">
         <v>8.2098</v>
@@ -1009,7 +1009,7 @@
         <v>8.062200000000001</v>
       </c>
       <c r="C41" t="n">
-        <v>8.062200000000001</v>
+        <v>8.139200000000001</v>
       </c>
       <c r="D41" t="n">
         <v>8.062200000000001</v>
@@ -1023,7 +1023,7 @@
         <v>8.0693</v>
       </c>
       <c r="C42" t="n">
-        <v>8.0693</v>
+        <v>8.0626</v>
       </c>
       <c r="D42" t="n">
         <v>8.0693</v>
@@ -1037,7 +1037,7 @@
         <v>8.055</v>
       </c>
       <c r="C43" t="n">
-        <v>8.055</v>
+        <v>7.9691</v>
       </c>
       <c r="D43" t="n">
         <v>8.055</v>
@@ -1051,7 +1051,7 @@
         <v>8.083600000000001</v>
       </c>
       <c r="C44" t="n">
-        <v>8.083600000000001</v>
+        <v>8.010199999999999</v>
       </c>
       <c r="D44" t="n">
         <v>8.083600000000001</v>
@@ -1065,7 +1065,7 @@
         <v>8.118399999999999</v>
       </c>
       <c r="C45" t="n">
-        <v>8.118399999999999</v>
+        <v>8.0258</v>
       </c>
       <c r="D45" t="n">
         <v>8.118399999999999</v>
@@ -1079,7 +1079,7 @@
         <v>8.0732</v>
       </c>
       <c r="C46" t="n">
-        <v>8.0732</v>
+        <v>8.0345</v>
       </c>
       <c r="D46" t="n">
         <v>8.0732</v>
@@ -1093,7 +1093,7 @@
         <v>7.9452</v>
       </c>
       <c r="C47" t="n">
-        <v>7.9452</v>
+        <v>7.9086</v>
       </c>
       <c r="D47" t="n">
         <v>7.9452</v>
@@ -1107,7 +1107,7 @@
         <v>7.8921</v>
       </c>
       <c r="C48" t="n">
-        <v>7.8921</v>
+        <v>7.8967</v>
       </c>
       <c r="D48" t="n">
         <v>7.8921</v>
@@ -1121,7 +1121,7 @@
         <v>7.9157</v>
       </c>
       <c r="C49" t="n">
-        <v>7.9157</v>
+        <v>7.8231</v>
       </c>
       <c r="D49" t="n">
         <v>7.9157</v>
@@ -1135,7 +1135,7 @@
         <v>8.0198</v>
       </c>
       <c r="C50" t="n">
-        <v>8.0198</v>
+        <v>8.0291</v>
       </c>
       <c r="D50" t="n">
         <v>8.0198</v>
@@ -1149,7 +1149,7 @@
         <v>7.79</v>
       </c>
       <c r="C51" t="n">
-        <v>7.79</v>
+        <v>7.8099</v>
       </c>
       <c r="D51" t="n">
         <v>7.79</v>
@@ -1163,7 +1163,7 @@
         <v>7.8245</v>
       </c>
       <c r="C52" t="n">
-        <v>7.8245</v>
+        <v>7.8046</v>
       </c>
       <c r="D52" t="n">
         <v>7.8245</v>
@@ -1177,7 +1177,7 @@
         <v>7.8685</v>
       </c>
       <c r="C53" t="n">
-        <v>7.8685</v>
+        <v>7.7844</v>
       </c>
       <c r="D53" t="n">
         <v>7.8685</v>
@@ -1191,7 +1191,7 @@
         <v>7.8404</v>
       </c>
       <c r="C54" t="n">
-        <v>7.8404</v>
+        <v>7.7735</v>
       </c>
       <c r="D54" t="n">
         <v>7.8404</v>
@@ -1205,7 +1205,7 @@
         <v>7.7621</v>
       </c>
       <c r="C55" t="n">
-        <v>7.7621</v>
+        <v>7.7738</v>
       </c>
       <c r="D55" t="n">
         <v>7.7621</v>
@@ -1219,7 +1219,7 @@
         <v>7.839</v>
       </c>
       <c r="C56" t="n">
-        <v>7.839</v>
+        <v>7.7904</v>
       </c>
       <c r="D56" t="n">
         <v>7.839</v>
@@ -1233,7 +1233,7 @@
         <v>7.7533</v>
       </c>
       <c r="C57" t="n">
-        <v>7.7533</v>
+        <v>7.8042</v>
       </c>
       <c r="D57" t="n">
         <v>7.7533</v>
@@ -1247,7 +1247,7 @@
         <v>7.7215</v>
       </c>
       <c r="C58" t="n">
-        <v>7.7215</v>
+        <v>7.6969</v>
       </c>
       <c r="D58" t="n">
         <v>7.7215</v>
@@ -1261,7 +1261,7 @@
         <v>7.7258</v>
       </c>
       <c r="C59" t="n">
-        <v>7.7258</v>
+        <v>7.6637</v>
       </c>
       <c r="D59" t="n">
         <v>7.7258</v>
@@ -1275,7 +1275,7 @@
         <v>7.6255</v>
       </c>
       <c r="C60" t="n">
-        <v>7.6255</v>
+        <v>7.6589</v>
       </c>
       <c r="D60" t="n">
         <v>7.6255</v>
@@ -1289,7 +1289,7 @@
         <v>7.7008</v>
       </c>
       <c r="C61" t="n">
-        <v>7.7008</v>
+        <v>7.6671</v>
       </c>
       <c r="D61" t="n">
         <v>7.7008</v>
@@ -1303,7 +1303,7 @@
         <v>7.6806</v>
       </c>
       <c r="C62" t="n">
-        <v>7.6806</v>
+        <v>7.6235</v>
       </c>
       <c r="D62" t="n">
         <v>7.6806</v>
@@ -1317,7 +1317,7 @@
         <v>7.6877</v>
       </c>
       <c r="C63" t="n">
-        <v>7.6877</v>
+        <v>7.7323</v>
       </c>
       <c r="D63" t="n">
         <v>7.6877</v>
@@ -1331,7 +1331,7 @@
         <v>7.5777</v>
       </c>
       <c r="C64" t="n">
-        <v>7.5777</v>
+        <v>7.6433</v>
       </c>
       <c r="D64" t="n">
         <v>7.5777</v>
@@ -1345,7 +1345,7 @@
         <v>7.5558</v>
       </c>
       <c r="C65" t="n">
-        <v>7.5558</v>
+        <v>7.5541</v>
       </c>
       <c r="D65" t="n">
         <v>7.5558</v>
@@ -1359,7 +1359,7 @@
         <v>7.5759</v>
       </c>
       <c r="C66" t="n">
-        <v>7.5759</v>
+        <v>7.6192</v>
       </c>
       <c r="D66" t="n">
         <v>7.5759</v>
@@ -1373,7 +1373,7 @@
         <v>7.5453</v>
       </c>
       <c r="C67" t="n">
-        <v>7.5453</v>
+        <v>7.5705</v>
       </c>
       <c r="D67" t="n">
         <v>7.5453</v>
@@ -1387,7 +1387,7 @@
         <v>7.5599</v>
       </c>
       <c r="C68" t="n">
-        <v>7.5599</v>
+        <v>7.5854</v>
       </c>
       <c r="D68" t="n">
         <v>7.5599</v>
@@ -1401,7 +1401,7 @@
         <v>7.5091</v>
       </c>
       <c r="C69" t="n">
-        <v>7.5091</v>
+        <v>7.5267</v>
       </c>
       <c r="D69" t="n">
         <v>7.5091</v>
@@ -1415,7 +1415,7 @@
         <v>7.6268</v>
       </c>
       <c r="C70" t="n">
-        <v>7.6268</v>
+        <v>7.6292</v>
       </c>
       <c r="D70" t="n">
         <v>7.6268</v>
@@ -1429,7 +1429,7 @@
         <v>7.5508</v>
       </c>
       <c r="C71" t="n">
-        <v>7.5508</v>
+        <v>7.5736</v>
       </c>
       <c r="D71" t="n">
         <v>7.5508</v>
@@ -1443,7 +1443,7 @@
         <v>7.5086</v>
       </c>
       <c r="C72" t="n">
-        <v>7.5086</v>
+        <v>7.5412</v>
       </c>
       <c r="D72" t="n">
         <v>7.5086</v>
@@ -1457,7 +1457,7 @@
         <v>7.523</v>
       </c>
       <c r="C73" t="n">
-        <v>7.523</v>
+        <v>7.5046</v>
       </c>
       <c r="D73" t="n">
         <v>7.523</v>
@@ -1471,7 +1471,7 @@
         <v>7.4811</v>
       </c>
       <c r="C74" t="n">
-        <v>7.4811</v>
+        <v>7.4838</v>
       </c>
       <c r="D74" t="n">
         <v>7.4811</v>
@@ -1485,7 +1485,7 @@
         <v>7.3686</v>
       </c>
       <c r="C75" t="n">
-        <v>7.3686</v>
+        <v>7.4096</v>
       </c>
       <c r="D75" t="n">
         <v>7.3686</v>
@@ -1499,7 +1499,7 @@
         <v>7.3739</v>
       </c>
       <c r="C76" t="n">
-        <v>7.3739</v>
+        <v>7.4085</v>
       </c>
       <c r="D76" t="n">
         <v>7.3739</v>
@@ -1513,7 +1513,7 @@
         <v>7.4073</v>
       </c>
       <c r="C77" t="n">
-        <v>7.4073</v>
+        <v>7.3907</v>
       </c>
       <c r="D77" t="n">
         <v>7.4073</v>
@@ -1527,7 +1527,7 @@
         <v>7.4357</v>
       </c>
       <c r="C78" t="n">
-        <v>7.4357</v>
+        <v>7.4885</v>
       </c>
       <c r="D78" t="n">
         <v>7.4357</v>
@@ -1541,7 +1541,7 @@
         <v>7.4363</v>
       </c>
       <c r="C79" t="n">
-        <v>7.4363</v>
+        <v>7.4924</v>
       </c>
       <c r="D79" t="n">
         <v>7.4363</v>
@@ -1555,7 +1555,7 @@
         <v>7.4685</v>
       </c>
       <c r="C80" t="n">
-        <v>7.4685</v>
+        <v>7.4182</v>
       </c>
       <c r="D80" t="n">
         <v>7.4685</v>
@@ -1569,7 +1569,7 @@
         <v>7.4433</v>
       </c>
       <c r="C81" t="n">
-        <v>7.4433</v>
+        <v>7.5339</v>
       </c>
       <c r="D81" t="n">
         <v>7.4433</v>
@@ -1583,7 +1583,7 @@
         <v>7.3968</v>
       </c>
       <c r="C82" t="n">
-        <v>7.3968</v>
+        <v>7.4137</v>
       </c>
       <c r="D82" t="n">
         <v>7.3968</v>
@@ -1597,7 +1597,7 @@
         <v>7.3817</v>
       </c>
       <c r="C83" t="n">
-        <v>7.3817</v>
+        <v>7.4612</v>
       </c>
       <c r="D83" t="n">
         <v>7.3817</v>
@@ -1611,7 +1611,7 @@
         <v>7.322</v>
       </c>
       <c r="C84" t="n">
-        <v>7.322</v>
+        <v>7.4139</v>
       </c>
       <c r="D84" t="n">
         <v>7.322</v>
@@ -1625,7 +1625,7 @@
         <v>7.4454</v>
       </c>
       <c r="C85" t="n">
-        <v>7.4454</v>
+        <v>7.4434</v>
       </c>
       <c r="D85" t="n">
         <v>7.4454</v>

</xml_diff>

<commit_message>
add table_chart script with postnorm
</commit_message>
<xml_diff>
--- a/visualization/perplexity_table.xlsx
+++ b/visualization/perplexity_table.xlsx
@@ -466,7 +466,7 @@
         <v>33.9126</v>
       </c>
       <c r="D2" t="n">
-        <v>36.7371</v>
+        <v>34.1502</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>26.7691</v>
       </c>
       <c r="D3" t="n">
-        <v>26.8323</v>
+        <v>26.359</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>23.2335</v>
       </c>
       <c r="D4" t="n">
-        <v>22.725</v>
+        <v>23.2081</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +508,7 @@
         <v>20.7174</v>
       </c>
       <c r="D5" t="n">
-        <v>20.6885</v>
+        <v>21.6382</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         <v>18.8327</v>
       </c>
       <c r="D6" t="n">
-        <v>19.0923</v>
+        <v>20.2516</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +536,7 @@
         <v>17.4664</v>
       </c>
       <c r="D7" t="n">
-        <v>17.8984</v>
+        <v>19.251</v>
       </c>
     </row>
     <row r="8">
@@ -550,7 +550,7 @@
         <v>16.0299</v>
       </c>
       <c r="D8" t="n">
-        <v>17.2346</v>
+        <v>18.6105</v>
       </c>
     </row>
     <row r="9">
@@ -564,7 +564,7 @@
         <v>14.7069</v>
       </c>
       <c r="D9" t="n">
-        <v>16.2702</v>
+        <v>18.0149</v>
       </c>
     </row>
     <row r="10">
@@ -578,7 +578,7 @@
         <v>13.1254</v>
       </c>
       <c r="D10" t="n">
-        <v>15.4719</v>
+        <v>17.4068</v>
       </c>
     </row>
     <row r="11">
@@ -592,7 +592,7 @@
         <v>12.2506</v>
       </c>
       <c r="D11" t="n">
-        <v>14.5493</v>
+        <v>16.9958</v>
       </c>
     </row>
     <row r="12">
@@ -606,7 +606,7 @@
         <v>11.582</v>
       </c>
       <c r="D12" t="n">
-        <v>13.5227</v>
+        <v>16.4747</v>
       </c>
     </row>
     <row r="13">
@@ -620,7 +620,7 @@
         <v>11.24</v>
       </c>
       <c r="D13" t="n">
-        <v>12.4982</v>
+        <v>16.1425</v>
       </c>
     </row>
     <row r="14">
@@ -634,7 +634,7 @@
         <v>10.8999</v>
       </c>
       <c r="D14" t="n">
-        <v>11.7911</v>
+        <v>15.9092</v>
       </c>
     </row>
     <row r="15">
@@ -648,7 +648,7 @@
         <v>10.4693</v>
       </c>
       <c r="D15" t="n">
-        <v>11.1716</v>
+        <v>15.3756</v>
       </c>
     </row>
     <row r="16">
@@ -662,7 +662,7 @@
         <v>10.2536</v>
       </c>
       <c r="D16" t="n">
-        <v>10.7728</v>
+        <v>15.1456</v>
       </c>
     </row>
     <row r="17">
@@ -676,7 +676,7 @@
         <v>9.966200000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>10.4022</v>
+        <v>14.5205</v>
       </c>
     </row>
     <row r="18">
@@ -690,7 +690,7 @@
         <v>9.8307</v>
       </c>
       <c r="D18" t="n">
-        <v>10.2219</v>
+        <v>14.1912</v>
       </c>
     </row>
     <row r="19">
@@ -704,7 +704,7 @@
         <v>9.6778</v>
       </c>
       <c r="D19" t="n">
-        <v>10.1277</v>
+        <v>13.7762</v>
       </c>
     </row>
     <row r="20">
@@ -718,7 +718,7 @@
         <v>9.592499999999999</v>
       </c>
       <c r="D20" t="n">
-        <v>9.918699999999999</v>
+        <v>13.3218</v>
       </c>
     </row>
     <row r="21">
@@ -732,7 +732,7 @@
         <v>9.424200000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>9.7295</v>
+        <v>12.9442</v>
       </c>
     </row>
     <row r="22">
@@ -746,7 +746,7 @@
         <v>9.3149</v>
       </c>
       <c r="D22" t="n">
-        <v>9.6303</v>
+        <v>12.4055</v>
       </c>
     </row>
     <row r="23">
@@ -760,7 +760,7 @@
         <v>9.076700000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>9.4011</v>
+        <v>11.902</v>
       </c>
     </row>
     <row r="24">
@@ -774,7 +774,7 @@
         <v>9.058</v>
       </c>
       <c r="D24" t="n">
-        <v>9.2904</v>
+        <v>11.4914</v>
       </c>
     </row>
     <row r="25">
@@ -788,7 +788,7 @@
         <v>8.942299999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>9.214499999999999</v>
+        <v>11.1672</v>
       </c>
     </row>
     <row r="26">
@@ -802,7 +802,7 @@
         <v>8.9269</v>
       </c>
       <c r="D26" t="n">
-        <v>9.0945</v>
+        <v>10.8755</v>
       </c>
     </row>
     <row r="27">
@@ -816,7 +816,7 @@
         <v>8.7235</v>
       </c>
       <c r="D27" t="n">
-        <v>8.9445</v>
+        <v>10.5402</v>
       </c>
     </row>
     <row r="28">
@@ -830,7 +830,7 @@
         <v>8.697900000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>8.965299999999999</v>
+        <v>10.4516</v>
       </c>
     </row>
     <row r="29">
@@ -844,7 +844,7 @@
         <v>8.5908</v>
       </c>
       <c r="D29" t="n">
-        <v>8.859</v>
+        <v>10.2334</v>
       </c>
     </row>
     <row r="30">
@@ -858,7 +858,7 @@
         <v>8.601100000000001</v>
       </c>
       <c r="D30" t="n">
-        <v>8.7577</v>
+        <v>10.0067</v>
       </c>
     </row>
     <row r="31">
@@ -872,7 +872,7 @@
         <v>8.539</v>
       </c>
       <c r="D31" t="n">
-        <v>8.667899999999999</v>
+        <v>9.890700000000001</v>
       </c>
     </row>
     <row r="32">
@@ -886,7 +886,7 @@
         <v>8.469099999999999</v>
       </c>
       <c r="D32" t="n">
-        <v>8.5959</v>
+        <v>9.738</v>
       </c>
     </row>
     <row r="33">
@@ -900,7 +900,7 @@
         <v>8.3421</v>
       </c>
       <c r="D33" t="n">
-        <v>8.487500000000001</v>
+        <v>9.543699999999999</v>
       </c>
     </row>
     <row r="34">
@@ -914,7 +914,7 @@
         <v>8.336399999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>8.4442</v>
+        <v>9.3931</v>
       </c>
     </row>
     <row r="35">
@@ -928,7 +928,7 @@
         <v>8.2117</v>
       </c>
       <c r="D35" t="n">
-        <v>8.3749</v>
+        <v>9.3147</v>
       </c>
     </row>
     <row r="36">
@@ -942,7 +942,7 @@
         <v>8.236800000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>8.3592</v>
+        <v>9.333600000000001</v>
       </c>
     </row>
     <row r="37">
@@ -956,7 +956,7 @@
         <v>8.3376</v>
       </c>
       <c r="D37" t="n">
-        <v>8.372</v>
+        <v>9.205500000000001</v>
       </c>
     </row>
     <row r="38">
@@ -970,7 +970,7 @@
         <v>8.2333</v>
       </c>
       <c r="D38" t="n">
-        <v>8.289899999999999</v>
+        <v>9.1509</v>
       </c>
     </row>
     <row r="39">
@@ -984,7 +984,7 @@
         <v>8.1289</v>
       </c>
       <c r="D39" t="n">
-        <v>8.1881</v>
+        <v>9.017200000000001</v>
       </c>
     </row>
     <row r="40">
@@ -998,7 +998,7 @@
         <v>8.2066</v>
       </c>
       <c r="D40" t="n">
-        <v>8.2098</v>
+        <v>9.0693</v>
       </c>
     </row>
     <row r="41">
@@ -1012,7 +1012,7 @@
         <v>8.139200000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>8.062200000000001</v>
+        <v>8.8813</v>
       </c>
     </row>
     <row r="42">
@@ -1026,7 +1026,7 @@
         <v>8.0626</v>
       </c>
       <c r="D42" t="n">
-        <v>8.0693</v>
+        <v>8.9475</v>
       </c>
     </row>
     <row r="43">
@@ -1040,7 +1040,7 @@
         <v>7.9691</v>
       </c>
       <c r="D43" t="n">
-        <v>8.055</v>
+        <v>8.788</v>
       </c>
     </row>
     <row r="44">
@@ -1054,7 +1054,7 @@
         <v>8.010199999999999</v>
       </c>
       <c r="D44" t="n">
-        <v>8.083600000000001</v>
+        <v>8.818300000000001</v>
       </c>
     </row>
     <row r="45">
@@ -1068,7 +1068,7 @@
         <v>8.0258</v>
       </c>
       <c r="D45" t="n">
-        <v>8.118399999999999</v>
+        <v>8.7014</v>
       </c>
     </row>
     <row r="46">
@@ -1082,7 +1082,7 @@
         <v>8.0345</v>
       </c>
       <c r="D46" t="n">
-        <v>8.0732</v>
+        <v>8.722</v>
       </c>
     </row>
     <row r="47">
@@ -1096,7 +1096,7 @@
         <v>7.9086</v>
       </c>
       <c r="D47" t="n">
-        <v>7.9452</v>
+        <v>8.642300000000001</v>
       </c>
     </row>
     <row r="48">
@@ -1110,7 +1110,7 @@
         <v>7.8967</v>
       </c>
       <c r="D48" t="n">
-        <v>7.8921</v>
+        <v>8.5817</v>
       </c>
     </row>
     <row r="49">
@@ -1124,7 +1124,7 @@
         <v>7.8231</v>
       </c>
       <c r="D49" t="n">
-        <v>7.9157</v>
+        <v>8.488099999999999</v>
       </c>
     </row>
     <row r="50">
@@ -1138,7 +1138,7 @@
         <v>8.0291</v>
       </c>
       <c r="D50" t="n">
-        <v>8.0198</v>
+        <v>8.644399999999999</v>
       </c>
     </row>
     <row r="51">
@@ -1152,7 +1152,7 @@
         <v>7.8099</v>
       </c>
       <c r="D51" t="n">
-        <v>7.79</v>
+        <v>8.428900000000001</v>
       </c>
     </row>
     <row r="52">
@@ -1166,7 +1166,7 @@
         <v>7.8046</v>
       </c>
       <c r="D52" t="n">
-        <v>7.8245</v>
+        <v>8.393599999999999</v>
       </c>
     </row>
     <row r="53">
@@ -1180,7 +1180,7 @@
         <v>7.7844</v>
       </c>
       <c r="D53" t="n">
-        <v>7.8685</v>
+        <v>8.4091</v>
       </c>
     </row>
     <row r="54">
@@ -1194,7 +1194,7 @@
         <v>7.7735</v>
       </c>
       <c r="D54" t="n">
-        <v>7.8404</v>
+        <v>8.416700000000001</v>
       </c>
     </row>
     <row r="55">
@@ -1208,7 +1208,7 @@
         <v>7.7738</v>
       </c>
       <c r="D55" t="n">
-        <v>7.7621</v>
+        <v>8.2903</v>
       </c>
     </row>
     <row r="56">
@@ -1222,7 +1222,7 @@
         <v>7.7904</v>
       </c>
       <c r="D56" t="n">
-        <v>7.839</v>
+        <v>8.2728</v>
       </c>
     </row>
     <row r="57">
@@ -1236,7 +1236,7 @@
         <v>7.8042</v>
       </c>
       <c r="D57" t="n">
-        <v>7.7533</v>
+        <v>8.278</v>
       </c>
     </row>
     <row r="58">
@@ -1250,7 +1250,7 @@
         <v>7.6969</v>
       </c>
       <c r="D58" t="n">
-        <v>7.7215</v>
+        <v>8.146000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -1264,7 +1264,7 @@
         <v>7.6637</v>
       </c>
       <c r="D59" t="n">
-        <v>7.7258</v>
+        <v>8.1754</v>
       </c>
     </row>
     <row r="60">
@@ -1278,7 +1278,7 @@
         <v>7.6589</v>
       </c>
       <c r="D60" t="n">
-        <v>7.6255</v>
+        <v>8.048500000000001</v>
       </c>
     </row>
     <row r="61">
@@ -1292,7 +1292,7 @@
         <v>7.6671</v>
       </c>
       <c r="D61" t="n">
-        <v>7.7008</v>
+        <v>8.1318</v>
       </c>
     </row>
     <row r="62">
@@ -1306,7 +1306,7 @@
         <v>7.6235</v>
       </c>
       <c r="D62" t="n">
-        <v>7.6806</v>
+        <v>8.139699999999999</v>
       </c>
     </row>
     <row r="63">
@@ -1320,7 +1320,7 @@
         <v>7.7323</v>
       </c>
       <c r="D63" t="n">
-        <v>7.6877</v>
+        <v>8.1144</v>
       </c>
     </row>
     <row r="64">
@@ -1334,7 +1334,7 @@
         <v>7.6433</v>
       </c>
       <c r="D64" t="n">
-        <v>7.5777</v>
+        <v>7.9396</v>
       </c>
     </row>
     <row r="65">
@@ -1348,7 +1348,7 @@
         <v>7.5541</v>
       </c>
       <c r="D65" t="n">
-        <v>7.5558</v>
+        <v>7.9627</v>
       </c>
     </row>
     <row r="66">
@@ -1362,7 +1362,7 @@
         <v>7.6192</v>
       </c>
       <c r="D66" t="n">
-        <v>7.5759</v>
+        <v>7.9509</v>
       </c>
     </row>
     <row r="67">
@@ -1376,7 +1376,7 @@
         <v>7.5705</v>
       </c>
       <c r="D67" t="n">
-        <v>7.5453</v>
+        <v>7.8626</v>
       </c>
     </row>
     <row r="68">
@@ -1390,7 +1390,7 @@
         <v>7.5854</v>
       </c>
       <c r="D68" t="n">
-        <v>7.5599</v>
+        <v>7.8828</v>
       </c>
     </row>
     <row r="69">
@@ -1404,7 +1404,7 @@
         <v>7.5267</v>
       </c>
       <c r="D69" t="n">
-        <v>7.5091</v>
+        <v>7.9132</v>
       </c>
     </row>
     <row r="70">
@@ -1418,7 +1418,7 @@
         <v>7.6292</v>
       </c>
       <c r="D70" t="n">
-        <v>7.6268</v>
+        <v>8.0014</v>
       </c>
     </row>
     <row r="71">
@@ -1432,7 +1432,7 @@
         <v>7.5736</v>
       </c>
       <c r="D71" t="n">
-        <v>7.5508</v>
+        <v>7.9219</v>
       </c>
     </row>
     <row r="72">
@@ -1446,7 +1446,7 @@
         <v>7.5412</v>
       </c>
       <c r="D72" t="n">
-        <v>7.5086</v>
+        <v>7.9201</v>
       </c>
     </row>
     <row r="73">
@@ -1460,7 +1460,7 @@
         <v>7.5046</v>
       </c>
       <c r="D73" t="n">
-        <v>7.523</v>
+        <v>7.8476</v>
       </c>
     </row>
     <row r="74">
@@ -1474,7 +1474,7 @@
         <v>7.4838</v>
       </c>
       <c r="D74" t="n">
-        <v>7.4811</v>
+        <v>7.838</v>
       </c>
     </row>
     <row r="75">
@@ -1488,7 +1488,7 @@
         <v>7.4096</v>
       </c>
       <c r="D75" t="n">
-        <v>7.3686</v>
+        <v>7.8439</v>
       </c>
     </row>
     <row r="76">
@@ -1502,7 +1502,7 @@
         <v>7.4085</v>
       </c>
       <c r="D76" t="n">
-        <v>7.3739</v>
+        <v>7.7219</v>
       </c>
     </row>
     <row r="77">
@@ -1516,7 +1516,7 @@
         <v>7.3907</v>
       </c>
       <c r="D77" t="n">
-        <v>7.4073</v>
+        <v>7.7787</v>
       </c>
     </row>
     <row r="78">
@@ -1530,7 +1530,7 @@
         <v>7.4885</v>
       </c>
       <c r="D78" t="n">
-        <v>7.4357</v>
+        <v>7.8238</v>
       </c>
     </row>
     <row r="79">
@@ -1544,7 +1544,7 @@
         <v>7.4924</v>
       </c>
       <c r="D79" t="n">
-        <v>7.4363</v>
+        <v>7.8293</v>
       </c>
     </row>
     <row r="80">
@@ -1558,7 +1558,7 @@
         <v>7.4182</v>
       </c>
       <c r="D80" t="n">
-        <v>7.4685</v>
+        <v>7.7649</v>
       </c>
     </row>
     <row r="81">
@@ -1572,7 +1572,7 @@
         <v>7.5339</v>
       </c>
       <c r="D81" t="n">
-        <v>7.4433</v>
+        <v>7.7102</v>
       </c>
     </row>
     <row r="82">
@@ -1586,7 +1586,7 @@
         <v>7.4137</v>
       </c>
       <c r="D82" t="n">
-        <v>7.3968</v>
+        <v>7.6923</v>
       </c>
     </row>
     <row r="83">
@@ -1600,7 +1600,7 @@
         <v>7.4612</v>
       </c>
       <c r="D83" t="n">
-        <v>7.3817</v>
+        <v>7.7038</v>
       </c>
     </row>
     <row r="84">
@@ -1614,7 +1614,7 @@
         <v>7.4139</v>
       </c>
       <c r="D84" t="n">
-        <v>7.322</v>
+        <v>7.6921</v>
       </c>
     </row>
     <row r="85">
@@ -1628,7 +1628,7 @@
         <v>7.4434</v>
       </c>
       <c r="D85" t="n">
-        <v>7.4454</v>
+        <v>7.6737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>